<commit_message>
wycinek rzeczywistosci, diagram erd
</commit_message>
<xml_diff>
--- a/Reguły i ograniczenia.xlsx
+++ b/Reguły i ograniczenia.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17626"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86e0a143b4b81594/Semestr V/Bazy Danych/Projekt/Bazy_Danych_Projekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Anna\OneDrive\Semestr V\Bazy Danych\Projekt\Bazy_Danych_Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1362B0EA-C7B8-4226-980D-651EC5C41ED5}" xr6:coauthVersionLast="12" xr6:coauthVersionMax="12" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27855" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16575" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="217">
   <si>
     <t>REG001</t>
   </si>
@@ -658,13 +657,31 @@
   </si>
   <si>
     <t xml:space="preserve">Metoda płatności musi przyjąć numer 1 i opis 'GOTOWKA' lub numer 2 i opis 'KARTA' lub numer 3 i opis 'CZEK' lub numer 4 i opis 'PRZELEW' </t>
+  </si>
+  <si>
+    <t>REG032</t>
+  </si>
+  <si>
+    <t>REG033</t>
+  </si>
+  <si>
+    <t>Gość może figurować w bazie jednocześnie nie wynajmując żadnego pokoju</t>
+  </si>
+  <si>
+    <t>Klient może figurować w bazie, nie dokonując jednocześnie żadnej rezerwacji</t>
+  </si>
+  <si>
+    <t>REG034</t>
+  </si>
+  <si>
+    <t>Klient może nie wybrać przez pewien czas żadnej metody płatności</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1009,19 +1026,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="137.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1037,7 +1054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1045,7 +1062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1053,7 +1070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1061,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1069,7 +1086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1085,7 +1102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1093,7 +1110,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1101,7 +1118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1109,7 +1126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1117,7 +1134,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1125,7 +1142,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1133,7 +1150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1141,7 +1158,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1149,7 +1166,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1157,7 +1174,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1165,7 +1182,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1173,7 +1190,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1181,7 +1198,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1189,7 +1206,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1197,7 +1214,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1205,7 +1222,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1213,7 +1230,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1221,7 +1238,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1229,7 +1246,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1237,7 +1254,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1245,7 +1262,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1253,7 +1270,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1261,7 +1278,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1269,611 +1286,635 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>78</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>80</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>82</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>88</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B49" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>90</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B50" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>92</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>94</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B52" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>96</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>98</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>100</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B55" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>102</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B56" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>104</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>106</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>108</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>109</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>110</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B61" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>112</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>114</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>116</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B64" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>118</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>120</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B66" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>122</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>124</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>126</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>128</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B70" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>130</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B71" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>132</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B72" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>134</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>136</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B74" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>138</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B75" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>140</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>142</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>144</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B78" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>146</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B79" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>148</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B80" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>150</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B81" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>152</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B82" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>154</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>156</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B84" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>158</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B85" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>160</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B86" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>162</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B87" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>164</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B88" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>166</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B89" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>168</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B90" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>170</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B91" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>172</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B92" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>174</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B93" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>176</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B94" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>177</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B95" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>179</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B96" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>181</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B97" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>183</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B98" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>185</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B99" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>187</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B100" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>189</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B101" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>191</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B102" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>193</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B103" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>195</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B104" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>197</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B105" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>199</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B106" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>201</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B107" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>203</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B108" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>205</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B109" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>207</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B110" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>209</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B111" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>